<commit_message>
Deleting the date 20170424_01_174_177 because data not usable (zero data apparently, cannot divide by 0 for log10 appliance).
</commit_message>
<xml_diff>
--- a/data/Exclusion_folder/data_2017_2018.xlsx
+++ b/data/Exclusion_folder/data_2017_2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\data\Exclusion_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D76502E-D785-43C7-9BE7-2316635088BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204381F7-3A00-4C9C-B25A-9AD0427FBE8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3590" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="189">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -589,6 +589,9 @@
   </si>
   <si>
     <t>20180501_02_137_138</t>
+  </si>
+  <si>
+    <t>deleted cause not usable!</t>
   </si>
 </sst>
 </file>
@@ -942,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD85FA16-C23A-4FBA-BF82-A4B483A385D3}">
   <dimension ref="A1:B166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="E162" sqref="E162"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1281,82 +1284,85 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
Deleted the dates '20170510_02_033_034' and '20170322_01_010_016' because they were not appropriate for processing.
</commit_message>
<xml_diff>
--- a/data/Exclusion_folder/data_2017_2018.xlsx
+++ b/data/Exclusion_folder/data_2017_2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\data\Exclusion_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204381F7-3A00-4C9C-B25A-9AD0427FBE8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C802A91D-D507-4626-B0A7-CEA1D65D7E70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3590" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3585" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="190">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -592,6 +592,9 @@
   </si>
   <si>
     <t>deleted cause not usable!</t>
+  </si>
+  <si>
+    <t>deleted because shitty</t>
   </si>
 </sst>
 </file>
@@ -945,32 +948,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD85FA16-C23A-4FBA-BF82-A4B483A385D3}">
   <dimension ref="A1:B166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.08984375" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -978,177 +984,177 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1156,72 +1162,72 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -1229,117 +1235,117 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>78</v>
       </c>
@@ -1347,47 +1353,47 @@
         <v>188</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -1395,27 +1401,27 @@
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -1423,47 +1429,47 @@
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>102</v>
       </c>
@@ -1471,27 +1477,30 @@
         <v>103</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B102" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>110</v>
       </c>
@@ -1499,7 +1508,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>111</v>
       </c>
@@ -1507,7 +1516,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>114</v>
       </c>
@@ -1515,7 +1524,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>115</v>
       </c>
@@ -1523,17 +1532,17 @@
         <v>116</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>119</v>
       </c>
@@ -1541,17 +1550,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>124</v>
       </c>
@@ -1559,27 +1568,27 @@
         <v>123</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>129</v>
       </c>
@@ -1587,17 +1596,17 @@
         <v>134</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>132</v>
       </c>
@@ -1605,7 +1614,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>135</v>
       </c>
@@ -1613,32 +1622,32 @@
         <v>120</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>141</v>
       </c>
@@ -1646,7 +1655,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>143</v>
       </c>
@@ -1654,22 +1663,22 @@
         <v>144</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>148</v>
       </c>
@@ -1677,27 +1686,27 @@
         <v>149</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>154</v>
       </c>
@@ -1705,7 +1714,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>156</v>
       </c>
@@ -1713,7 +1722,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>158</v>
       </c>
@@ -1721,102 +1730,102 @@
         <v>159</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>179</v>
       </c>
@@ -1824,7 +1833,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>181</v>
       </c>
@@ -1832,7 +1841,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>183</v>
       </c>
@@ -1840,17 +1849,17 @@
         <v>184</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>187</v>
       </c>

</xml_diff>

<commit_message>
Elongating the 2018 traces.
</commit_message>
<xml_diff>
--- a/data/Exclusion_folder/data_2017_2018.xlsx
+++ b/data/Exclusion_folder/data_2017_2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\data\Exclusion_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C802A91D-D507-4626-B0A7-CEA1D65D7E70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FB3448-D6BC-4046-AD73-7E67B0828107}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3585" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3590" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,15 +405,9 @@
     <t>20170511_01_176_178</t>
   </si>
   <si>
-    <t>20180404_02_002_003</t>
-  </si>
-  <si>
     <t>20180404_02_005_006</t>
   </si>
   <si>
-    <t>20180405_01_004_005</t>
-  </si>
-  <si>
     <t>20180405_01_008_012</t>
   </si>
   <si>
@@ -435,24 +429,15 @@
     <t>20180405_01_063_064</t>
   </si>
   <si>
-    <t>20180405_01_079_082</t>
-  </si>
-  <si>
     <t>20180405_01_085_087</t>
   </si>
   <si>
     <t>20180405_01_090_091</t>
   </si>
   <si>
-    <t>20180405_01_134_135</t>
-  </si>
-  <si>
     <t>20180405_01_160_161</t>
   </si>
   <si>
-    <t>20180418_01_001_002</t>
-  </si>
-  <si>
     <t>ended at 001</t>
   </si>
   <si>
@@ -465,12 +450,6 @@
     <t>20180419_02_032_033</t>
   </si>
   <si>
-    <t>20180419_02_036_036</t>
-  </si>
-  <si>
-    <t>20180419_02_040_042</t>
-  </si>
-  <si>
     <t>20180419_02_056_072</t>
   </si>
   <si>
@@ -483,9 +462,6 @@
     <t>20180419_02_113_114</t>
   </si>
   <si>
-    <t>20180419_02_125_126</t>
-  </si>
-  <si>
     <t>20180419_02_128_128</t>
   </si>
   <si>
@@ -513,12 +489,6 @@
     <t>20180423_01_056_056</t>
   </si>
   <si>
-    <t>20180423_01_093_093</t>
-  </si>
-  <si>
-    <t>20180423_01_100_100</t>
-  </si>
-  <si>
     <t>20180423_01_109_109</t>
   </si>
   <si>
@@ -534,9 +504,6 @@
     <t>20180426_01_004_006</t>
   </si>
   <si>
-    <t>20180426_01_018_018</t>
-  </si>
-  <si>
     <t>20180427_01_004_006</t>
   </si>
   <si>
@@ -555,9 +522,6 @@
     <t>20180430_01_015_018</t>
   </si>
   <si>
-    <t>20180430_01_030_030</t>
-  </si>
-  <si>
     <t>20180430_01_074_077</t>
   </si>
   <si>
@@ -595,6 +559,42 @@
   </si>
   <si>
     <t>deleted because shitty</t>
+  </si>
+  <si>
+    <t>20180404_02_002_004</t>
+  </si>
+  <si>
+    <t>20180405_01_004_006</t>
+  </si>
+  <si>
+    <t>20180405_01_078_082</t>
+  </si>
+  <si>
+    <t>20180405_01_134_136</t>
+  </si>
+  <si>
+    <t>20180418_01_001_003</t>
+  </si>
+  <si>
+    <t>20180419_02_035_036</t>
+  </si>
+  <si>
+    <t>20180419_02_040_043</t>
+  </si>
+  <si>
+    <t>20180419_02_123_126</t>
+  </si>
+  <si>
+    <t>20180423_01_093_094</t>
+  </si>
+  <si>
+    <t>20180423_01_097_100</t>
+  </si>
+  <si>
+    <t>20180426_01_016_018</t>
+  </si>
+  <si>
+    <t>20180430_01_030_032</t>
   </si>
 </sst>
 </file>
@@ -948,35 +948,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD85FA16-C23A-4FBA-BF82-A4B483A385D3}">
   <dimension ref="A1:B166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="A158" sqref="A158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -984,177 +984,177 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1162,72 +1162,72 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -1235,165 +1235,165 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -1401,27 +1401,27 @@
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -1429,47 +1429,47 @@
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>102</v>
       </c>
@@ -1477,30 +1477,30 @@
         <v>103</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>107</v>
       </c>
       <c r="B102" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>110</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>111</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>114</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>115</v>
       </c>
@@ -1532,17 +1532,17 @@
         <v>116</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>119</v>
       </c>
@@ -1550,17 +1550,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>124</v>
       </c>
@@ -1568,300 +1568,300 @@
         <v>123</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="B119" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
         <v>129</v>
       </c>
-      <c r="B119" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="B122" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>132</v>
-      </c>
-      <c r="B122" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>135</v>
       </c>
       <c r="B123" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>182</v>
+      </c>
+      <c r="B129" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="B130" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
         <v>141</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B134" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
         <v>143</v>
       </c>
-      <c r="B130" t="s">
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="B139" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
         <v>148</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B140" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+      <c r="B141" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
         <v>154</v>
       </c>
-      <c r="B139" t="s">
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
         <v>156</v>
       </c>
-      <c r="B140" t="s">
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
         <v>158</v>
       </c>
-      <c r="B141" t="s">
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="B161" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+      <c r="B162" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+      <c r="B163" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>179</v>
-      </c>
-      <c r="B161" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>181</v>
-      </c>
-      <c r="B162" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>183</v>
-      </c>
-      <c r="B163" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merging 20180404_02_002_004 with 20180404_02_005_006, making the trace 20180404_02_002_006.
</commit_message>
<xml_diff>
--- a/data/Exclusion_folder/data_2017_2018.xlsx
+++ b/data/Exclusion_folder/data_2017_2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\data\Exclusion_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FB3448-D6BC-4046-AD73-7E67B0828107}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F77FB5-69A8-4DB2-BB86-179DFB283BAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3590" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="189">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -405,9 +405,6 @@
     <t>20170511_01_176_178</t>
   </si>
   <si>
-    <t>20180404_02_005_006</t>
-  </si>
-  <si>
     <t>20180405_01_008_012</t>
   </si>
   <si>
@@ -561,9 +558,6 @@
     <t>deleted because shitty</t>
   </si>
   <si>
-    <t>20180404_02_002_004</t>
-  </si>
-  <si>
     <t>20180405_01_004_006</t>
   </si>
   <si>
@@ -595,6 +589,9 @@
   </si>
   <si>
     <t>20180430_01_030_032</t>
+  </si>
+  <si>
+    <t>20180404_02_002_006</t>
   </si>
 </sst>
 </file>
@@ -946,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD85FA16-C23A-4FBA-BF82-A4B483A385D3}">
-  <dimension ref="A1:B166"/>
+  <dimension ref="A1:B165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="A158" sqref="A158"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117:XFD117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -968,7 +965,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1350,7 +1347,7 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
@@ -1492,7 +1489,7 @@
         <v>107</v>
       </c>
       <c r="B102" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -1575,26 +1572,26 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>126</v>
+        <v>177</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>179</v>
+        <v>126</v>
+      </c>
+      <c r="B118" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>127</v>
       </c>
-      <c r="B119" t="s">
-        <v>132</v>
-      </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
@@ -1605,26 +1602,26 @@
       <c r="A121" t="s">
         <v>129</v>
       </c>
+      <c r="B121" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B122" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>133</v>
-      </c>
-      <c r="B123" t="s">
-        <v>120</v>
+        <v>178</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>180</v>
+        <v>133</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
@@ -1634,55 +1631,55 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>135</v>
+        <v>179</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>181</v>
+        <v>135</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
+        <v>180</v>
+      </c>
+      <c r="B128" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>182</v>
+        <v>137</v>
       </c>
       <c r="B129" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>138</v>
-      </c>
-      <c r="B130" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>140</v>
+        <v>181</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>184</v>
+        <v>140</v>
+      </c>
+      <c r="B133" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>141</v>
-      </c>
-      <c r="B134" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1693,40 +1690,40 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>145</v>
       </c>
+      <c r="B138" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B139" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B140" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>150</v>
-      </c>
-      <c r="B141" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1737,115 +1734,115 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>153</v>
+        <v>184</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A151" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A158" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>166</v>
       </c>
+      <c r="B160" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B161" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B162" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>171</v>
-      </c>
-      <c r="B163" t="s">
         <v>172</v>
       </c>
     </row>
@@ -1857,11 +1854,6 @@
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A166" t="s">
-        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prolonging the following traces: 20180419_02_040_044, 20180405_01_134_137, 20180418_01_001_004, 20180423_01_095_100.
</commit_message>
<xml_diff>
--- a/data/Exclusion_folder/data_2017_2018.xlsx
+++ b/data/Exclusion_folder/data_2017_2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\data\Exclusion_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F77FB5-69A8-4DB2-BB86-179DFB283BAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10933FF8-728F-42CB-AFA8-9B613F676BC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3590" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
   </bookViews>
@@ -564,27 +564,15 @@
     <t>20180405_01_078_082</t>
   </si>
   <si>
-    <t>20180405_01_134_136</t>
-  </si>
-  <si>
-    <t>20180418_01_001_003</t>
-  </si>
-  <si>
     <t>20180419_02_035_036</t>
   </si>
   <si>
-    <t>20180419_02_040_043</t>
-  </si>
-  <si>
     <t>20180419_02_123_126</t>
   </si>
   <si>
     <t>20180423_01_093_094</t>
   </si>
   <si>
-    <t>20180423_01_097_100</t>
-  </si>
-  <si>
     <t>20180426_01_016_018</t>
   </si>
   <si>
@@ -592,6 +580,18 @@
   </si>
   <si>
     <t>20180404_02_002_006</t>
+  </si>
+  <si>
+    <t>20180419_02_040_044</t>
+  </si>
+  <si>
+    <t>20180405_01_134_137</t>
+  </si>
+  <si>
+    <t>20180418_01_001_004</t>
+  </si>
+  <si>
+    <t>20180423_01_095_100</t>
   </si>
 </sst>
 </file>
@@ -945,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD85FA16-C23A-4FBA-BF82-A4B483A385D3}">
   <dimension ref="A1:B165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117:XFD117"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1572,7 +1572,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
@@ -1631,7 +1631,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
@@ -1641,7 +1641,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="B128" t="s">
         <v>136</v>
@@ -1662,12 +1662,12 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
@@ -1690,7 +1690,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
@@ -1734,12 +1734,12 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -1769,7 +1769,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
@@ -1804,7 +1804,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Merging '20180423_01_093_094' with '20180423_01_095_100' making '20180423_01_093_100'.
</commit_message>
<xml_diff>
--- a/data/Exclusion_folder/data_2017_2018.xlsx
+++ b/data/Exclusion_folder/data_2017_2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\data\Exclusion_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10933FF8-728F-42CB-AFA8-9B613F676BC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E84D95-5DA2-43C3-B856-B499F085F78E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3590" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="188">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -570,9 +570,6 @@
     <t>20180419_02_123_126</t>
   </si>
   <si>
-    <t>20180423_01_093_094</t>
-  </si>
-  <si>
     <t>20180426_01_016_018</t>
   </si>
   <si>
@@ -591,7 +588,7 @@
     <t>20180418_01_001_004</t>
   </si>
   <si>
-    <t>20180423_01_095_100</t>
+    <t>20180423_01_093_100</t>
   </si>
 </sst>
 </file>
@@ -943,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD85FA16-C23A-4FBA-BF82-A4B483A385D3}">
-  <dimension ref="A1:B165"/>
+  <dimension ref="A1:B164"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
+      <selection activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1572,7 +1569,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
@@ -1631,7 +1628,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
@@ -1641,7 +1638,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B128" t="s">
         <v>136</v>
@@ -1667,7 +1664,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
@@ -1734,125 +1731,120 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="B159" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B160" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B161" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>170</v>
-      </c>
-      <c r="B162" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A165" t="s">
         <v>174</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deleting '20170327_04_106_106' because signal is bad.
</commit_message>
<xml_diff>
--- a/data/Exclusion_folder/data_2017_2018.xlsx
+++ b/data/Exclusion_folder/data_2017_2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\data\Exclusion_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E84D95-5DA2-43C3-B856-B499F085F78E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CFD5F0-97D6-487C-A868-8E2E34D1FFD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3590" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="189">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -589,6 +589,9 @@
   </si>
   <si>
     <t>20180423_01_093_100</t>
+  </si>
+  <si>
+    <t>deleted because signal is shitty</t>
   </si>
 </sst>
 </file>
@@ -942,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD85FA16-C23A-4FBA-BF82-A4B483A385D3}">
   <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="B142" sqref="B142"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1007,6 +1010,9 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="B10" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
Finishing 2017 exclusion affining.
</commit_message>
<xml_diff>
--- a/data/Exclusion_folder/data_2017_2018.xlsx
+++ b/data/Exclusion_folder/data_2017_2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\data\Exclusion_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CFD5F0-97D6-487C-A868-8E2E34D1FFD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EF3B29-E9D8-4F4A-8624-46935B3A56A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3590" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>20170322_03_001_001</t>
   </si>
   <si>
-    <t>check quickly</t>
-  </si>
-  <si>
     <t>20170327_04_034_035</t>
   </si>
   <si>
@@ -592,6 +589,9 @@
   </si>
   <si>
     <t>deleted because signal is shitty</t>
+  </si>
+  <si>
+    <t>deleted because no ice slabs in it</t>
   </si>
 </sst>
 </file>
@@ -946,7 +946,7 @@
   <dimension ref="A1:B164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -965,7 +965,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -978,880 +978,880 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
         <v>39</v>
-      </c>
-      <c r="B39" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
         <v>54</v>
-      </c>
-      <c r="B53" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85" t="s">
         <v>87</v>
-      </c>
-      <c r="B85" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>92</v>
+      </c>
+      <c r="B90" t="s">
         <v>93</v>
-      </c>
-      <c r="B90" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
+        <v>101</v>
+      </c>
+      <c r="B99" t="s">
         <v>102</v>
-      </c>
-      <c r="B99" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B102" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B104" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
+        <v>110</v>
+      </c>
+      <c r="B105" t="s">
         <v>111</v>
-      </c>
-      <c r="B105" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B106" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
+        <v>114</v>
+      </c>
+      <c r="B107" t="s">
         <v>115</v>
-      </c>
-      <c r="B107" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
+        <v>118</v>
+      </c>
+      <c r="B110" t="s">
         <v>119</v>
-      </c>
-      <c r="B110" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B113" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B118" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
+        <v>128</v>
+      </c>
+      <c r="B121" t="s">
         <v>129</v>
-      </c>
-      <c r="B121" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B122" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B128" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
+        <v>136</v>
+      </c>
+      <c r="B129" t="s">
         <v>137</v>
-      </c>
-      <c r="B129" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
+        <v>139</v>
+      </c>
+      <c r="B133" t="s">
         <v>140</v>
-      </c>
-      <c r="B133" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
+        <v>144</v>
+      </c>
+      <c r="B138" t="s">
         <v>145</v>
-      </c>
-      <c r="B138" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
+        <v>146</v>
+      </c>
+      <c r="B139" t="s">
         <v>147</v>
-      </c>
-      <c r="B139" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
+        <v>148</v>
+      </c>
+      <c r="B140" t="s">
         <v>149</v>
-      </c>
-      <c r="B140" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
+        <v>165</v>
+      </c>
+      <c r="B159" t="s">
         <v>166</v>
-      </c>
-      <c r="B159" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
+        <v>167</v>
+      </c>
+      <c r="B160" t="s">
         <v>168</v>
-      </c>
-      <c r="B160" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
+        <v>169</v>
+      </c>
+      <c r="B161" t="s">
         <v>170</v>
-      </c>
-      <c r="B161" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleting 20180419_02_016_018 because no ice slabs in it.
</commit_message>
<xml_diff>
--- a/data/Exclusion_folder/data_2017_2018.xlsx
+++ b/data/Exclusion_folder/data_2017_2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\data\Exclusion_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EF3B29-E9D8-4F4A-8624-46935B3A56A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DF9D19-BD01-4B70-91AB-669E89D8F1CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3590" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
   </bookViews>
@@ -438,9 +438,6 @@
     <t>20180419_02_016_018</t>
   </si>
   <si>
-    <t>a added them</t>
-  </si>
-  <si>
     <t>20180419_02_032_033</t>
   </si>
   <si>
@@ -592,6 +589,9 @@
   </si>
   <si>
     <t>deleted because no ice slabs in it</t>
+  </si>
+  <si>
+    <t>deleted</t>
   </si>
 </sst>
 </file>
@@ -945,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD85FA16-C23A-4FBA-BF82-A4B483A385D3}">
   <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -965,7 +965,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -978,7 +978,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1011,7 +1011,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1350,7 +1350,7 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
@@ -1492,7 +1492,7 @@
         <v>106</v>
       </c>
       <c r="B102" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -1575,12 +1575,12 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -1619,7 +1619,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -1634,7 +1634,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
@@ -1644,7 +1644,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B128" t="s">
         <v>135</v>
@@ -1655,203 +1655,203 @@
         <v>136</v>
       </c>
       <c r="B129" t="s">
-        <v>137</v>
+        <v>188</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
+        <v>138</v>
+      </c>
+      <c r="B133" t="s">
         <v>139</v>
-      </c>
-      <c r="B133" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
+        <v>143</v>
+      </c>
+      <c r="B138" t="s">
         <v>144</v>
-      </c>
-      <c r="B138" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
+        <v>145</v>
+      </c>
+      <c r="B139" t="s">
         <v>146</v>
-      </c>
-      <c r="B139" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
+        <v>147</v>
+      </c>
+      <c r="B140" t="s">
         <v>148</v>
-      </c>
-      <c r="B140" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
+        <v>164</v>
+      </c>
+      <c r="B159" t="s">
         <v>165</v>
-      </c>
-      <c r="B159" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
+        <v>166</v>
+      </c>
+      <c r="B160" t="s">
         <v>167</v>
-      </c>
-      <c r="B160" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
+        <v>168</v>
+      </c>
+      <c r="B161" t="s">
         <v>169</v>
-      </c>
-      <c r="B161" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2018 exclusion affining and removal of 20180429_01_179_181 because periodicity not manageable.
</commit_message>
<xml_diff>
--- a/data/Exclusion_folder/data_2017_2018.xlsx
+++ b/data/Exclusion_folder/data_2017_2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\data\Exclusion_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DF9D19-BD01-4B70-91AB-669E89D8F1CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB598BB2-769A-482A-88DA-17CABF16411B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3590" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="190">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -592,6 +592,9 @@
   </si>
   <si>
     <t>deleted</t>
+  </si>
+  <si>
+    <t>periodicity not manageable</t>
   </si>
 </sst>
 </file>
@@ -945,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD85FA16-C23A-4FBA-BF82-A4B483A385D3}">
   <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="D132" sqref="D132"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1794,6 +1797,9 @@
       <c r="A154" t="s">
         <v>160</v>
       </c>
+      <c r="B154" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">

</xml_diff>

<commit_message>
Re-adding 20180405_01_004_006 to check the periodicity issue by comparing with Li Jilu's email.
</commit_message>
<xml_diff>
--- a/data/Exclusion_folder/data_2017_2018.xlsx
+++ b/data/Exclusion_folder/data_2017_2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\data\Exclusion_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB598BB2-769A-482A-88DA-17CABF16411B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60F7438-8B90-4732-9CB4-8BCCDCE57199}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3590" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="191">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -595,6 +595,9 @@
   </si>
   <si>
     <t>periodicity not manageable</t>
+  </si>
+  <si>
+    <t>readded</t>
   </si>
 </sst>
 </file>
@@ -948,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD85FA16-C23A-4FBA-BF82-A4B483A385D3}">
   <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1585,6 +1588,9 @@
       <c r="A117" t="s">
         <v>175</v>
       </c>
+      <c r="B117" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">

</xml_diff>

<commit_message>
Affining 2018 data that were not affined yet before because they experienced periodicity issue. As I now have a solution to correct for the periodicity of the signal (cf. previous commit), I am not able to work with these data and thus I did this round of affining 2018 data.
</commit_message>
<xml_diff>
--- a/data/Exclusion_folder/data_2017_2018.xlsx
+++ b/data/Exclusion_folder/data_2017_2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\data\Exclusion_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60F7438-8B90-4732-9CB4-8BCCDCE57199}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015F151B-9860-4CAF-A183-5F2E0AB76ABF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3590" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3585" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="192">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -598,6 +598,9 @@
   </si>
   <si>
     <t>readded</t>
+  </si>
+  <si>
+    <t>deleted because no ice slabs</t>
   </si>
 </sst>
 </file>
@@ -952,21 +955,21 @@
   <dimension ref="A1:B164"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+      <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -974,12 +977,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -987,32 +990,32 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1020,147 +1023,147 @@
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1168,72 +1171,72 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1241,117 +1244,117 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>77</v>
       </c>
@@ -1359,47 +1362,47 @@
         <v>173</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>86</v>
       </c>
@@ -1407,27 +1410,27 @@
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>92</v>
       </c>
@@ -1435,47 +1438,47 @@
         <v>93</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>101</v>
       </c>
@@ -1483,17 +1486,17 @@
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>106</v>
       </c>
@@ -1501,12 +1504,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>109</v>
       </c>
@@ -1514,7 +1517,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>110</v>
       </c>
@@ -1522,7 +1525,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>113</v>
       </c>
@@ -1530,7 +1533,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>114</v>
       </c>
@@ -1538,17 +1541,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>118</v>
       </c>
@@ -1556,17 +1559,17 @@
         <v>119</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>123</v>
       </c>
@@ -1574,17 +1577,17 @@
         <v>122</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>175</v>
       </c>
@@ -1592,7 +1595,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>125</v>
       </c>
@@ -1600,17 +1603,17 @@
         <v>130</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>128</v>
       </c>
@@ -1618,7 +1621,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>131</v>
       </c>
@@ -1626,32 +1629,32 @@
         <v>119</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>184</v>
       </c>
@@ -1659,7 +1662,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>136</v>
       </c>
@@ -1667,22 +1670,22 @@
         <v>188</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>138</v>
       </c>
@@ -1690,27 +1693,30 @@
         <v>139</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B135" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>143</v>
       </c>
@@ -1718,7 +1724,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>145</v>
       </c>
@@ -1726,7 +1732,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>147</v>
       </c>
@@ -1734,72 +1740,72 @@
         <v>148</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>160</v>
       </c>
@@ -1807,27 +1813,27 @@
         <v>189</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>164</v>
       </c>
@@ -1835,7 +1841,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>166</v>
       </c>
@@ -1843,7 +1849,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>168</v>
       </c>
@@ -1851,17 +1857,17 @@
         <v>169</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>172</v>
       </c>

</xml_diff>

<commit_message>
Very last affining of 2017 and 2018 data. These data are now ready to work with! Deleted 20170510_02_088_093 because noisy signal.
</commit_message>
<xml_diff>
--- a/data/Exclusion_folder/data_2017_2018.xlsx
+++ b/data/Exclusion_folder/data_2017_2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\data\Exclusion_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015F151B-9860-4CAF-A183-5F2E0AB76ABF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F510440E-644B-4B2C-A67D-05B6DA6B2041}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3585" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3590" xr2:uid="{9DCE4092-96C4-44BD-9C3D-9192ECC5DF51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,9 +363,6 @@
     <t>ended at 083</t>
   </si>
   <si>
-    <t>started at 089</t>
-  </si>
-  <si>
     <t>20170510_02_088_093</t>
   </si>
   <si>
@@ -601,6 +598,9 @@
   </si>
   <si>
     <t>deleted because no ice slabs</t>
+  </si>
+  <si>
+    <t>deleted cause noisy</t>
   </si>
 </sst>
 </file>
@@ -954,216 +954,216 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD85FA16-C23A-4FBA-BF82-A4B483A385D3}">
   <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="D136" sqref="D136"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1171,72 +1171,72 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1244,165 +1244,165 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>86</v>
       </c>
@@ -1410,27 +1410,27 @@
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>92</v>
       </c>
@@ -1438,47 +1438,47 @@
         <v>93</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>101</v>
       </c>
@@ -1486,30 +1486,30 @@
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>106</v>
       </c>
       <c r="B102" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>109</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>110</v>
       </c>
@@ -1525,351 +1525,351 @@
         <v>111</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
+        <v>112</v>
+      </c>
+      <c r="B106" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>113</v>
       </c>
-      <c r="B106" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="B107" t="s">
         <v>114</v>
       </c>
-      <c r="B107" t="s">
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="B110" t="s">
         <v>118</v>
       </c>
-      <c r="B110" t="s">
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>122</v>
+      </c>
+      <c r="B113" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
         <v>123</v>
       </c>
-      <c r="B113" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>174</v>
+      </c>
+      <c r="B117" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="B118" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>127</v>
+      </c>
+      <c r="B121" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>130</v>
+      </c>
+      <c r="B122" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>183</v>
+      </c>
+      <c r="B128" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>135</v>
+      </c>
+      <c r="B129" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>175</v>
-      </c>
-      <c r="B117" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>137</v>
+      </c>
+      <c r="B133" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>140</v>
+      </c>
+      <c r="B135" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>125</v>
-      </c>
-      <c r="B118" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>128</v>
-      </c>
-      <c r="B121" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>131</v>
-      </c>
-      <c r="B122" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>142</v>
+      </c>
+      <c r="B138" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>144</v>
+      </c>
+      <c r="B139" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>146</v>
+      </c>
+      <c r="B140" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
         <v>184</v>
       </c>
-      <c r="B128" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>136</v>
-      </c>
-      <c r="B129" t="s">
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>159</v>
+      </c>
+      <c r="B154" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>138</v>
-      </c>
-      <c r="B133" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>141</v>
-      </c>
-      <c r="B135" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>143</v>
-      </c>
-      <c r="B138" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>145</v>
-      </c>
-      <c r="B139" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>147</v>
-      </c>
-      <c r="B140" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>160</v>
-      </c>
-      <c r="B154" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+      <c r="B159" t="s">
         <v>164</v>
       </c>
-      <c r="B159" t="s">
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+      <c r="B160" t="s">
         <v>166</v>
       </c>
-      <c r="B160" t="s">
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+      <c r="B161" t="s">
         <v>168</v>
       </c>
-      <c r="B161" t="s">
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>